<commit_message>
added cities database (Israel city list.xlsx) and import the database into a list of cities
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -742,47 +742,47 @@
       </c>
       <c r="B2" s="9">
         <f t="shared" ref="B2:C7" ca="1" si="0">RANDBETWEEN(200,80000)</f>
-        <v>70133</v>
+        <v>47893</v>
       </c>
       <c r="C2" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>16447</v>
+        <v>35624</v>
       </c>
       <c r="D2" s="9">
         <f t="shared" ref="D2:D7" ca="1" si="1">B2+C2</f>
-        <v>86580</v>
+        <v>83517</v>
       </c>
       <c r="E2" s="9">
         <f t="shared" ref="E2:I7" ca="1" si="2">RANDBETWEEN(200,80000)</f>
-        <v>52132</v>
+        <v>66121</v>
       </c>
       <c r="F2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>48106</v>
+        <v>4790</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>66993</v>
+        <v>9244</v>
       </c>
       <c r="H2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>50563</v>
+        <v>34915</v>
       </c>
       <c r="I2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>79501</v>
+        <v>8259</v>
       </c>
       <c r="J2" s="9">
         <f t="shared" ref="J2:J7" ca="1" si="3">(D2/M2)*1000000</f>
-        <v>412901.13359435729</v>
+        <v>398293.64719796652</v>
       </c>
       <c r="K2" s="9">
         <f t="shared" ref="K2:K7" ca="1" si="4">(I2/M2)*1000000</f>
-        <v>379141.29154406331</v>
+        <v>39387.27722748668</v>
       </c>
       <c r="L2" s="9">
         <f t="shared" ref="L2:L7" ca="1" si="5">(E2/M2)*1000000</f>
-        <v>248618.17852322749</v>
+        <v>315331.8994501328</v>
       </c>
       <c r="M2" s="10">
         <v>209687</v>
@@ -794,47 +794,47 @@
       </c>
       <c r="B3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>46758</v>
+        <v>43299</v>
       </c>
       <c r="C3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>29413</v>
+        <v>7659</v>
       </c>
       <c r="D3" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>76171</v>
+        <v>50958</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2927</v>
+        <v>39321</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1980</v>
+        <v>3777</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>73208</v>
+        <v>28008</v>
       </c>
       <c r="H3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>28687</v>
+        <v>13252</v>
       </c>
       <c r="I3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>34771</v>
+        <v>21925</v>
       </c>
       <c r="J3" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>165368.75858909759</v>
+        <v>110630.83325915682</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>75488.533758274294</v>
+        <v>47599.611821637685</v>
       </c>
       <c r="L3" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>6354.5753159376745</v>
+        <v>85366.674409971063</v>
       </c>
       <c r="M3" s="10">
         <v>460613</v>
@@ -846,47 +846,47 @@
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45715</v>
+        <v>9928</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>29607</v>
+        <v>42582</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>75322</v>
+        <v>52510</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>34919</v>
+        <v>13106</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>46412</v>
+        <v>54036</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>65357</v>
+        <v>9520</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>34088</v>
+        <v>9005</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>52572</v>
+        <v>71428</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>460738.55677418166</v>
+        <v>321199.40543549403</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>321578.65440020553</v>
+        <v>436919.27502278553</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>213596.68707678566</v>
+        <v>80168.337604981614</v>
       </c>
       <c r="M4" s="10">
         <v>163481</v>
@@ -898,47 +898,47 @@
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>68351</v>
+        <v>30375</v>
       </c>
       <c r="C5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>53510</v>
+        <v>38001</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>121861</v>
+        <v>68376</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>35309</v>
+        <v>75072</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>66145</v>
+        <v>17561</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>15928</v>
+        <v>23201</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>21926</v>
+        <v>22769</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>40695</v>
+        <v>67106</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>11838061.006411502</v>
+        <v>6642315.9121818533</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>3953273.7517000195</v>
+        <v>6518943.0736351274</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3430056.3435010687</v>
+        <v>7292791.9176219152</v>
       </c>
       <c r="M5" s="11">
         <v>10294</v>
@@ -950,47 +950,47 @@
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>29431</v>
+        <v>8083</v>
       </c>
       <c r="C6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>79793</v>
+        <v>24482</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>109224</v>
+        <v>32565</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>41708</v>
+        <v>35904</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>20069</v>
+        <v>1250</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>29471</v>
+        <v>58773</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>10696</v>
+        <v>27074</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>11363</v>
+        <v>38764</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>3166004.8117336738</v>
+        <v>943940.40406968317</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>329371.86585118412</v>
+        <v>1123626.7717904868</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1208962.5786254674</v>
+        <v>1040725.8181396561</v>
       </c>
       <c r="M6" s="10">
         <v>34499</v>
@@ -1002,47 +1002,47 @@
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>68359</v>
+        <v>63406</v>
       </c>
       <c r="C7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>17432</v>
+        <v>44141</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>85791</v>
+        <v>107547</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>41290</v>
+        <v>37666</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>71195</v>
+        <v>48592</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>40632</v>
+        <v>74975</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3006</v>
+        <v>46166</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>71713</v>
+        <v>28259</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>880178.51646660501</v>
+        <v>1103385.6571252693</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>735744.33158920694</v>
+        <v>289925.10516056226</v>
       </c>
       <c r="L7" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>423617.52334051504</v>
+        <v>386436.85236483021</v>
       </c>
       <c r="M7" s="10">
         <v>97470</v>
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
changed CovidConfirmMessage.py to communicate with AddPatientToDB.py changed New_Patient data class
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>City</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Patient Status</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>lasto</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -722,47 +731,47 @@
       </c>
       <c r="B2" s="9">
         <f t="shared" ref="B2:C7" ca="1" si="0">RANDBETWEEN(200,80000)</f>
-        <v>25264</v>
+        <v>9928</v>
       </c>
       <c r="C2" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>57002</v>
+        <v>33710</v>
       </c>
       <c r="D2" s="9">
         <f t="shared" ref="D2:D7" ca="1" si="1">B2+C2</f>
-        <v>82266</v>
+        <v>43638</v>
       </c>
       <c r="E2" s="9">
         <f t="shared" ref="E2:I7" ca="1" si="2">RANDBETWEEN(200,80000)</f>
-        <v>69465</v>
+        <v>26587</v>
       </c>
       <c r="F2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>40260</v>
+        <v>52387</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>48519</v>
+        <v>68525</v>
       </c>
       <c r="H2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>76844</v>
+        <v>46923</v>
       </c>
       <c r="I2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>71200</v>
+        <v>19230</v>
       </c>
       <c r="J2" s="9">
         <f t="shared" ref="J2:J7" ca="1" si="3">(D2/M2)*1000000</f>
-        <v>392327.61210756982</v>
+        <v>208110.18327316429</v>
       </c>
       <c r="K2" s="9">
         <f t="shared" ref="K2:K7" ca="1" si="4">(I2/M2)*1000000</f>
-        <v>339553.71577637142</v>
+        <v>91708.117336792464</v>
       </c>
       <c r="L2" s="9">
         <f t="shared" ref="L2:L7" ca="1" si="5">(E2/M2)*1000000</f>
-        <v>331279.47846075339</v>
+        <v>126793.74496273015</v>
       </c>
       <c r="M2" s="10">
         <v>209687</v>
@@ -774,47 +783,47 @@
       </c>
       <c r="B3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>36117</v>
+        <v>79434</v>
       </c>
       <c r="C3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>2239</v>
+        <v>51079</v>
       </c>
       <c r="D3" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>38356</v>
+        <v>130513</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>56936</v>
+        <v>7348</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>21095</v>
+        <v>6975</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>57500</v>
+        <v>59561</v>
       </c>
       <c r="H3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>12957</v>
+        <v>66650</v>
       </c>
       <c r="I3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>12878</v>
+        <v>7848</v>
       </c>
       <c r="J3" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>83271.64018384197</v>
+        <v>283346.32326920866</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>27958.394574187008</v>
+        <v>17038.164359234324</v>
       </c>
       <c r="L3" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>123609.19036153995</v>
+        <v>15952.654397509408</v>
       </c>
       <c r="M3" s="10">
         <v>460613</v>
@@ -826,47 +835,47 @@
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>15576</v>
+        <v>54084</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>63846</v>
+        <v>1862</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>79422</v>
+        <v>55946</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>65316</v>
+        <v>73230</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>47364</v>
+        <v>37529</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>10699</v>
+        <v>40968</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>72988</v>
+        <v>78138</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>29615</v>
+        <v>24284</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>485817.92379542574</v>
+        <v>342217.13838305365</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>181152.54983759578</v>
+        <v>148543.25579119287</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>399532.66740477487</v>
+        <v>447941.96267456154</v>
       </c>
       <c r="M4" s="10">
         <v>163481</v>
@@ -878,47 +887,47 @@
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>16130</v>
+        <v>48911</v>
       </c>
       <c r="C5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>8994</v>
+        <v>34200</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>25124</v>
+        <v>83111</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>69605</v>
+        <v>22322</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>64481</v>
+        <v>55089</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>44740</v>
+        <v>35246</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>18432</v>
+        <v>75881</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>24600</v>
+        <v>44196</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>2440645.0359432679</v>
+        <v>8073732.2712259572</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>2389741.5970468232</v>
+        <v>4293374.7814260731</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>6761705.8480668347</v>
+        <v>2168447.6394015932</v>
       </c>
       <c r="M5" s="11">
         <v>10294</v>
@@ -930,47 +939,47 @@
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45763</v>
+        <v>13831</v>
       </c>
       <c r="C6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>32519</v>
+        <v>1419</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>78282</v>
+        <v>15250</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>43792</v>
+        <v>77063</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>39475</v>
+        <v>29150</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2105</v>
+        <v>46785</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2131</v>
+        <v>61971</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>11710</v>
+        <v>54507</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>2269109.2495434647</v>
+        <v>442041.79831299454</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>339430.12840951915</v>
+        <v>1579958.8393866487</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1269370.1266703382</v>
+        <v>2233774.8920258558</v>
       </c>
       <c r="M6" s="10">
         <v>34499</v>
@@ -982,47 +991,47 @@
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>77538</v>
+        <v>21870</v>
       </c>
       <c r="C7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>29173</v>
+        <v>70039</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>106711</v>
+        <v>91909</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>37104</v>
+        <v>59563</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>28281</v>
+        <v>52577</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>65236</v>
+        <v>21484</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>48567</v>
+        <v>36648</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>72098</v>
+        <v>25519</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>1094808.659074587</v>
+        <v>942946.54765568895</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>739694.26490202115</v>
+        <v>261813.89145378064</v>
       </c>
       <c r="L7" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>380670.97568482609</v>
+        <v>611090.59197701851</v>
       </c>
       <c r="M7" s="10">
         <v>97470</v>
@@ -1518,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1563,12 +1572,24 @@
       <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>546827551</v>
+      </c>
+      <c r="D2" s="20">
+        <v>35028</v>
+      </c>
+      <c r="E2" s="20">
+        <v>44037</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="4"/>
@@ -1780,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
AddPatientToDB.py added method to open a new city sheet in the xlsx database if the city is not there
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Beer Sheva" sheetId="2" r:id="rId2"/>
     <sheet name="Tel Aviv" sheetId="3" r:id="rId3"/>
+    <sheet name="Yavne" sheetId="4" r:id="rId4"/>
+    <sheet name="Ashdod" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>City</t>
   </si>
@@ -336,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -381,6 +383,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,47 +736,47 @@
       </c>
       <c r="B2" s="9">
         <f t="shared" ref="B2:C7" ca="1" si="0">RANDBETWEEN(200,80000)</f>
-        <v>9928</v>
+        <v>70309</v>
       </c>
       <c r="C2" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>33710</v>
+        <v>60518</v>
       </c>
       <c r="D2" s="9">
         <f t="shared" ref="D2:D7" ca="1" si="1">B2+C2</f>
-        <v>43638</v>
+        <v>130827</v>
       </c>
       <c r="E2" s="9">
         <f t="shared" ref="E2:I7" ca="1" si="2">RANDBETWEEN(200,80000)</f>
-        <v>26587</v>
+        <v>76085</v>
       </c>
       <c r="F2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>52387</v>
+        <v>48630</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>68525</v>
+        <v>45823</v>
       </c>
       <c r="H2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>46923</v>
+        <v>79869</v>
       </c>
       <c r="I2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>19230</v>
+        <v>20541</v>
       </c>
       <c r="J2" s="9">
         <f t="shared" ref="J2:J7" ca="1" si="3">(D2/M2)*1000000</f>
-        <v>208110.18327316429</v>
+        <v>623915.64570049639</v>
       </c>
       <c r="K2" s="9">
         <f t="shared" ref="K2:K7" ca="1" si="4">(I2/M2)*1000000</f>
-        <v>91708.117336792464</v>
+        <v>97960.293198910746</v>
       </c>
       <c r="L2" s="9">
         <f t="shared" ref="L2:L7" ca="1" si="5">(E2/M2)*1000000</f>
-        <v>126793.74496273015</v>
+        <v>362850.34360737674</v>
       </c>
       <c r="M2" s="10">
         <v>209687</v>
@@ -783,47 +788,47 @@
       </c>
       <c r="B3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>79434</v>
+        <v>64069</v>
       </c>
       <c r="C3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>51079</v>
+        <v>62437</v>
       </c>
       <c r="D3" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>130513</v>
+        <v>126506</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>7348</v>
+        <v>66459</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>6975</v>
+        <v>68638</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>59561</v>
+        <v>38593</v>
       </c>
       <c r="H3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>66650</v>
+        <v>12765</v>
       </c>
       <c r="I3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>7848</v>
+        <v>68204</v>
       </c>
       <c r="J3" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>283346.32326920866</v>
+        <v>274647.04643594514</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>17038.164359234324</v>
+        <v>148072.24285897272</v>
       </c>
       <c r="L3" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>15952.654397509408</v>
+        <v>144283.81309255277</v>
       </c>
       <c r="M3" s="10">
         <v>460613</v>
@@ -835,47 +840,47 @@
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>54084</v>
+        <v>28716</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>1862</v>
+        <v>41995</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>55946</v>
+        <v>70711</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>73230</v>
+        <v>29570</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>37529</v>
+        <v>69647</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>40968</v>
+        <v>29475</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>78138</v>
+        <v>60746</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>24284</v>
+        <v>65455</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>342217.13838305365</v>
+        <v>432533.44425346062</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>148543.25579119287</v>
+        <v>400382.91911598289</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>447941.96267456154</v>
+        <v>180877.28849224068</v>
       </c>
       <c r="M4" s="10">
         <v>163481</v>
@@ -887,47 +892,47 @@
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>48911</v>
+        <v>40327</v>
       </c>
       <c r="C5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>34200</v>
+        <v>60104</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>83111</v>
+        <v>100431</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>22322</v>
+        <v>69609</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>55089</v>
+        <v>63726</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>35246</v>
+        <v>11988</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>75881</v>
+        <v>39080</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>44196</v>
+        <v>65027</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>8073732.2712259572</v>
+        <v>9756265.7858946957</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>4293374.7814260731</v>
+        <v>6316980.7654944621</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2168447.6394015932</v>
+        <v>6762094.4239362739</v>
       </c>
       <c r="M5" s="11">
         <v>10294</v>
@@ -939,47 +944,47 @@
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>13831</v>
+        <v>63867</v>
       </c>
       <c r="C6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>1419</v>
+        <v>10226</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>15250</v>
+        <v>74093</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>77063</v>
+        <v>50352</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>29150</v>
+        <v>72335</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>46785</v>
+        <v>61243</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>61971</v>
+        <v>30841</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>54507</v>
+        <v>22964</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>442041.79831299454</v>
+        <v>2147685.4401576859</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>1579958.8393866487</v>
+        <v>665642.48239079397</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2233774.8920258558</v>
+        <v>1459520.5658135018</v>
       </c>
       <c r="M6" s="10">
         <v>34499</v>
@@ -991,47 +996,47 @@
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>21870</v>
+        <v>2588</v>
       </c>
       <c r="C7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>70039</v>
+        <v>70305</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>91909</v>
+        <v>72893</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>59563</v>
+        <v>74946</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>52577</v>
+        <v>64901</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>21484</v>
+        <v>3262</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>36648</v>
+        <v>55474</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>25519</v>
+        <v>1171</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>942946.54765568895</v>
+        <v>747850.62070380629</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>261813.89145378064</v>
+        <v>12013.953011182928</v>
       </c>
       <c r="L7" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>611090.59197701851</v>
+        <v>768913.51184979989</v>
       </c>
       <c r="M7" s="10">
         <v>97470</v>
@@ -1527,7 +1532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -1801,15 +1806,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1836,12 +1841,24 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="24">
+        <v>546827551</v>
+      </c>
+      <c r="D2" s="20">
+        <v>35028</v>
+      </c>
+      <c r="E2" s="20">
+        <v>44037</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4"/>
@@ -2045,6 +2062,260 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="22">
+        <v>546827551</v>
+      </c>
+      <c r="D2" s="23">
+        <v>35028</v>
+      </c>
+      <c r="E2" s="23">
+        <v>44037</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="22">
+        <v>546827551</v>
+      </c>
+      <c r="D2" s="23">
+        <v>35028</v>
+      </c>
+      <c r="E2" s="23">
+        <v>44037</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added notes to AddPatientToDB.py and CovidConfirmMessage.py
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -736,47 +736,47 @@
       </c>
       <c r="B2" s="9">
         <f t="shared" ref="B2:C7" ca="1" si="0">RANDBETWEEN(200,80000)</f>
-        <v>70309</v>
+        <v>66379</v>
       </c>
       <c r="C2" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>60518</v>
+        <v>7416</v>
       </c>
       <c r="D2" s="9">
         <f t="shared" ref="D2:D7" ca="1" si="1">B2+C2</f>
-        <v>130827</v>
+        <v>73795</v>
       </c>
       <c r="E2" s="9">
         <f t="shared" ref="E2:I7" ca="1" si="2">RANDBETWEEN(200,80000)</f>
-        <v>76085</v>
+        <v>24409</v>
       </c>
       <c r="F2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>48630</v>
+        <v>32416</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>45823</v>
+        <v>38187</v>
       </c>
       <c r="H2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>79869</v>
+        <v>61256</v>
       </c>
       <c r="I2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>20541</v>
+        <v>42064</v>
       </c>
       <c r="J2" s="9">
         <f t="shared" ref="J2:J7" ca="1" si="3">(D2/M2)*1000000</f>
-        <v>623915.64570049639</v>
+        <v>351929.3041533333</v>
       </c>
       <c r="K2" s="9">
         <f t="shared" ref="K2:K7" ca="1" si="4">(I2/M2)*1000000</f>
-        <v>97960.293198910746</v>
+        <v>200603.75702833271</v>
       </c>
       <c r="L2" s="9">
         <f t="shared" ref="L2:L7" ca="1" si="5">(E2/M2)*1000000</f>
-        <v>362850.34360737674</v>
+        <v>116406.83494923386</v>
       </c>
       <c r="M2" s="10">
         <v>209687</v>
@@ -788,47 +788,47 @@
       </c>
       <c r="B3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>64069</v>
+        <v>49237</v>
       </c>
       <c r="C3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>62437</v>
+        <v>70758</v>
       </c>
       <c r="D3" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>126506</v>
+        <v>119995</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>66459</v>
+        <v>55132</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>68638</v>
+        <v>29655</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>38593</v>
+        <v>61638</v>
       </c>
       <c r="H3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>12765</v>
+        <v>73310</v>
       </c>
       <c r="I3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>68204</v>
+        <v>9066</v>
       </c>
       <c r="J3" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>274647.04643594514</v>
+        <v>260511.53571436324</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>148072.24285897272</v>
+        <v>19682.466625996225</v>
       </c>
       <c r="L3" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>144283.81309255277</v>
+        <v>119692.67041963644</v>
       </c>
       <c r="M3" s="10">
         <v>460613</v>
@@ -840,47 +840,47 @@
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>28716</v>
+        <v>6477</v>
       </c>
       <c r="C4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>41995</v>
+        <v>74578</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>70711</v>
+        <v>81055</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>29570</v>
+        <v>39619</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>69647</v>
+        <v>23029</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>29475</v>
+        <v>54399</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>60746</v>
+        <v>18754</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>65455</v>
+        <v>2069</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>432533.44425346062</v>
+        <v>495806.85217242368</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>400382.91911598289</v>
+        <v>12655.904967549746</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>180877.28849224068</v>
+        <v>242346.20536943129</v>
       </c>
       <c r="M4" s="10">
         <v>163481</v>
@@ -892,47 +892,47 @@
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>40327</v>
+        <v>9691</v>
       </c>
       <c r="C5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>60104</v>
+        <v>40326</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>100431</v>
+        <v>50017</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>69609</v>
+        <v>4575</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>63726</v>
+        <v>61528</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>11988</v>
+        <v>28492</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>39080</v>
+        <v>45136</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>65027</v>
+        <v>57042</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>9756265.7858946957</v>
+        <v>4858849.8154264614</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>6316980.7654944621</v>
+        <v>5541286.1861278415</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>6762094.4239362739</v>
+        <v>444433.65067029337</v>
       </c>
       <c r="M5" s="11">
         <v>10294</v>
@@ -944,47 +944,47 @@
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>63867</v>
+        <v>13550</v>
       </c>
       <c r="C6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>10226</v>
+        <v>50126</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>74093</v>
+        <v>63676</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>50352</v>
+        <v>43743</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>72335</v>
+        <v>34193</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>61243</v>
+        <v>72042</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>30841</v>
+        <v>29456</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>22964</v>
+        <v>17446</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>2147685.4401576859</v>
+        <v>1845734.6589756224</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>665642.48239079397</v>
+        <v>505695.81727006583</v>
       </c>
       <c r="L6" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1459520.5658135018</v>
+        <v>1267949.7956462507</v>
       </c>
       <c r="M6" s="10">
         <v>34499</v>
@@ -996,47 +996,47 @@
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>2588</v>
+        <v>77273</v>
       </c>
       <c r="C7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>70305</v>
+        <v>70468</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>72893</v>
+        <v>147741</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>74946</v>
+        <v>75923</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>64901</v>
+        <v>34309</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3262</v>
+        <v>75006</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>55474</v>
+        <v>72081</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1171</v>
+        <v>10877</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" ca="1" si="3"/>
-        <v>747850.62070380629</v>
+        <v>1515758.6949830716</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>12013.953011182928</v>
+        <v>111593.31076228584</v>
       </c>
       <c r="L7" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>768913.51184979989</v>
+        <v>778937.10885400639</v>
       </c>
       <c r="M7" s="10">
         <v>97470</v>
@@ -1807,7 +1807,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1817,7 +1817,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
in AddPatientToDB.py added format cell function to format date and ID cells
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="95">
   <si>
     <t>City</t>
   </si>
@@ -313,6 +313,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -538,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -586,6 +589,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
@@ -2298,7 +2303,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="5"/>
     </row>
-    <row r="74" spans="1:13" ht="15.75" thickBot="1">
+    <row r="74" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
       <c r="A74" s="6" t="s">
         <v>85</v>
       </c>
@@ -2326,7 +2331,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2379,10 +2384,10 @@
       <c r="C2" s="1">
         <v>546827551</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="25">
         <v>35028</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="25">
         <v>44037</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -2390,203 +2395,215 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1">
+        <v>546827551</v>
+      </c>
+      <c r="D3" s="25">
+        <v>35028</v>
+      </c>
+      <c r="E3" s="25">
+        <v>44037</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="4"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="4"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="4"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="4"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="4"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="8"/>
     </row>
   </sheetData>
@@ -2863,8 +2880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added Quarantine data (is Quarantined and where)
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="2" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8055" windowWidth="21570" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8055" windowWidth="21570" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Beersheba" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Tel Aviv-Yafo" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Ashdod" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="lod" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Lod" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21,7 +21,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt formatCode="m/d/yyyy;@" numFmtId="164"/>
-    <numFmt formatCode="DD-MM-YYYY" numFmtId="165"/>
+    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -248,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -293,11 +293,10 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -648,7 +647,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="23"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="11.7109375"/>
@@ -2278,10 +2277,10 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A1" sqref="A1:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="11.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="11.140625"/>
@@ -2289,8 +2288,8 @@
     <col bestFit="1" customWidth="1" max="4" min="4" width="13.42578125"/>
     <col bestFit="1" customWidth="1" max="5" min="5" width="12.7109375"/>
     <col bestFit="1" customWidth="1" max="6" min="6" width="17"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="11.42578125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="13.5703125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="20.5703125"/>
     <col bestFit="1" customWidth="1" max="9" min="9" width="24.42578125"/>
     <col bestFit="1" customWidth="1" max="10" min="10" width="24.140625"/>
     <col bestFit="1" customWidth="1" max="11" min="11" width="26.140625"/>
@@ -2322,13 +2321,21 @@
           <t>Test date</t>
         </is>
       </c>
-      <c r="F1" s="19" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>Patient Status</t>
         </is>
       </c>
-      <c r="G1" s="17" t="n"/>
-      <c r="H1" s="17" t="n"/>
+      <c r="G1" s="12" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="H1" s="19" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
       <c r="I1" s="17" t="n"/>
       <c r="J1" s="17" t="n"/>
       <c r="K1" s="17" t="n"/>
@@ -2347,17 +2354,19 @@
       <c r="C2" s="1" t="n">
         <v>546827551</v>
       </c>
-      <c r="D2" s="25" t="n">
+      <c r="D2" s="23" t="n">
         <v>35028</v>
       </c>
-      <c r="E2" s="25" t="n">
+      <c r="E2" s="23" t="n">
         <v>44037</v>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="5" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -2373,209 +2382,259 @@
       <c r="C3" s="1" t="n">
         <v>546827551</v>
       </c>
-      <c r="D3" s="25" t="n">
+      <c r="D3" s="23" t="n">
         <v>35028</v>
       </c>
-      <c r="E3" s="25" t="n">
+      <c r="E3" s="23" t="n">
         <v>44037</v>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="n"/>
       <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
-      <c r="D4" s="25" t="n"/>
-      <c r="E4" s="25" t="n"/>
-      <c r="F4" s="5" t="n"/>
+      <c r="D4" s="23" t="n"/>
+      <c r="E4" s="23" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n"/>
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
-      <c r="D5" s="25" t="n"/>
-      <c r="E5" s="25" t="n"/>
-      <c r="F5" s="5" t="n"/>
+      <c r="D5" s="23" t="n"/>
+      <c r="E5" s="23" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n"/>
       <c r="B6" s="1" t="n"/>
       <c r="C6" s="1" t="n"/>
-      <c r="D6" s="25" t="n"/>
-      <c r="E6" s="25" t="n"/>
-      <c r="F6" s="5" t="n"/>
+      <c r="D6" s="23" t="n"/>
+      <c r="E6" s="23" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n"/>
       <c r="B7" s="1" t="n"/>
       <c r="C7" s="1" t="n"/>
-      <c r="D7" s="25" t="n"/>
-      <c r="E7" s="25" t="n"/>
-      <c r="F7" s="5" t="n"/>
+      <c r="D7" s="23" t="n"/>
+      <c r="E7" s="23" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n"/>
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="n"/>
-      <c r="D8" s="25" t="n"/>
-      <c r="E8" s="25" t="n"/>
-      <c r="F8" s="5" t="n"/>
+      <c r="D8" s="23" t="n"/>
+      <c r="E8" s="23" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n"/>
-      <c r="D9" s="25" t="n"/>
-      <c r="E9" s="25" t="n"/>
-      <c r="F9" s="5" t="n"/>
+      <c r="D9" s="23" t="n"/>
+      <c r="E9" s="23" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="5" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="n"/>
       <c r="B10" s="1" t="n"/>
       <c r="C10" s="1" t="n"/>
-      <c r="D10" s="25" t="n"/>
-      <c r="E10" s="25" t="n"/>
-      <c r="F10" s="5" t="n"/>
+      <c r="D10" s="23" t="n"/>
+      <c r="E10" s="23" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="5" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n"/>
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
-      <c r="D11" s="25" t="n"/>
-      <c r="E11" s="25" t="n"/>
-      <c r="F11" s="5" t="n"/>
+      <c r="D11" s="23" t="n"/>
+      <c r="E11" s="23" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="5" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n"/>
       <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
-      <c r="D12" s="25" t="n"/>
-      <c r="E12" s="25" t="n"/>
-      <c r="F12" s="5" t="n"/>
+      <c r="D12" s="23" t="n"/>
+      <c r="E12" s="23" t="n"/>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n"/>
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
-      <c r="D13" s="25" t="n"/>
-      <c r="E13" s="25" t="n"/>
-      <c r="F13" s="5" t="n"/>
+      <c r="D13" s="23" t="n"/>
+      <c r="E13" s="23" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="5" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="n"/>
       <c r="B14" s="1" t="n"/>
       <c r="C14" s="1" t="n"/>
-      <c r="D14" s="25" t="n"/>
-      <c r="E14" s="25" t="n"/>
-      <c r="F14" s="5" t="n"/>
+      <c r="D14" s="23" t="n"/>
+      <c r="E14" s="23" t="n"/>
+      <c r="F14" s="1" t="n"/>
+      <c r="G14" s="1" t="n"/>
+      <c r="H14" s="5" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n"/>
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="n"/>
-      <c r="D15" s="25" t="n"/>
-      <c r="E15" s="25" t="n"/>
-      <c r="F15" s="5" t="n"/>
+      <c r="D15" s="23" t="n"/>
+      <c r="E15" s="23" t="n"/>
+      <c r="F15" s="1" t="n"/>
+      <c r="G15" s="1" t="n"/>
+      <c r="H15" s="5" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n"/>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="n"/>
-      <c r="D16" s="25" t="n"/>
-      <c r="E16" s="25" t="n"/>
-      <c r="F16" s="5" t="n"/>
+      <c r="D16" s="23" t="n"/>
+      <c r="E16" s="23" t="n"/>
+      <c r="F16" s="1" t="n"/>
+      <c r="G16" s="1" t="n"/>
+      <c r="H16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n"/>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="n"/>
-      <c r="D17" s="25" t="n"/>
-      <c r="E17" s="25" t="n"/>
-      <c r="F17" s="5" t="n"/>
+      <c r="D17" s="23" t="n"/>
+      <c r="E17" s="23" t="n"/>
+      <c r="F17" s="1" t="n"/>
+      <c r="G17" s="1" t="n"/>
+      <c r="H17" s="5" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="n"/>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n"/>
-      <c r="D18" s="25" t="n"/>
-      <c r="E18" s="25" t="n"/>
-      <c r="F18" s="5" t="n"/>
+      <c r="D18" s="23" t="n"/>
+      <c r="E18" s="23" t="n"/>
+      <c r="F18" s="1" t="n"/>
+      <c r="G18" s="1" t="n"/>
+      <c r="H18" s="5" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n"/>
       <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="n"/>
-      <c r="D19" s="25" t="n"/>
-      <c r="E19" s="25" t="n"/>
-      <c r="F19" s="5" t="n"/>
+      <c r="D19" s="23" t="n"/>
+      <c r="E19" s="23" t="n"/>
+      <c r="F19" s="1" t="n"/>
+      <c r="G19" s="1" t="n"/>
+      <c r="H19" s="5" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="n"/>
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="n"/>
-      <c r="D20" s="25" t="n"/>
-      <c r="E20" s="25" t="n"/>
-      <c r="F20" s="5" t="n"/>
+      <c r="D20" s="23" t="n"/>
+      <c r="E20" s="23" t="n"/>
+      <c r="F20" s="1" t="n"/>
+      <c r="G20" s="1" t="n"/>
+      <c r="H20" s="5" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n"/>
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="n"/>
-      <c r="D21" s="25" t="n"/>
-      <c r="E21" s="25" t="n"/>
-      <c r="F21" s="5" t="n"/>
+      <c r="D21" s="23" t="n"/>
+      <c r="E21" s="23" t="n"/>
+      <c r="F21" s="1" t="n"/>
+      <c r="G21" s="1" t="n"/>
+      <c r="H21" s="5" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="n"/>
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="n"/>
-      <c r="D22" s="25" t="n"/>
-      <c r="E22" s="25" t="n"/>
-      <c r="F22" s="5" t="n"/>
+      <c r="D22" s="23" t="n"/>
+      <c r="E22" s="23" t="n"/>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" s="1" t="n"/>
+      <c r="H22" s="5" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n"/>
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="n"/>
-      <c r="D23" s="25" t="n"/>
-      <c r="E23" s="25" t="n"/>
-      <c r="F23" s="5" t="n"/>
+      <c r="D23" s="23" t="n"/>
+      <c r="E23" s="23" t="n"/>
+      <c r="F23" s="1" t="n"/>
+      <c r="G23" s="1" t="n"/>
+      <c r="H23" s="5" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="n"/>
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="n"/>
-      <c r="D24" s="25" t="n"/>
-      <c r="E24" s="25" t="n"/>
-      <c r="F24" s="5" t="n"/>
+      <c r="D24" s="23" t="n"/>
+      <c r="E24" s="23" t="n"/>
+      <c r="F24" s="1" t="n"/>
+      <c r="G24" s="1" t="n"/>
+      <c r="H24" s="5" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n"/>
       <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="n"/>
-      <c r="D25" s="25" t="n"/>
-      <c r="E25" s="25" t="n"/>
-      <c r="F25" s="5" t="n"/>
+      <c r="D25" s="23" t="n"/>
+      <c r="E25" s="23" t="n"/>
+      <c r="F25" s="1" t="n"/>
+      <c r="G25" s="1" t="n"/>
+      <c r="H25" s="5" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n"/>
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="n"/>
-      <c r="D26" s="25" t="n"/>
-      <c r="E26" s="25" t="n"/>
-      <c r="F26" s="5" t="n"/>
+      <c r="D26" s="23" t="n"/>
+      <c r="E26" s="23" t="n"/>
+      <c r="F26" s="1" t="n"/>
+      <c r="G26" s="1" t="n"/>
+      <c r="H26" s="5" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="27" thickBot="1">
       <c r="A27" s="6" t="n"/>
       <c r="B27" s="7" t="n"/>
       <c r="C27" s="7" t="n"/>
-      <c r="D27" s="26" t="n"/>
-      <c r="E27" s="26" t="n"/>
-      <c r="F27" s="8" t="n"/>
+      <c r="D27" s="24" t="n"/>
+      <c r="E27" s="24" t="n"/>
+      <c r="F27" s="7" t="n"/>
+      <c r="G27" s="7" t="n"/>
+      <c r="H27" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2589,13 +2648,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="10.5703125"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="10.28515625"/>
@@ -2603,6 +2662,8 @@
     <col bestFit="1" customWidth="1" max="4" min="4" width="10.85546875"/>
     <col bestFit="1" customWidth="1" max="5" min="5" width="10"/>
     <col bestFit="1" customWidth="1" max="6" min="6" width="15"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="13.28515625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="20.5703125"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.75" r="1">
@@ -2631,9 +2692,19 @@
           <t>Test date</t>
         </is>
       </c>
-      <c r="F1" s="19" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>Patient Status</t>
+        </is>
+      </c>
+      <c r="G1" s="12" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="H1" s="19" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
         </is>
       </c>
     </row>
@@ -2648,7 +2719,7 @@
           <t>lasto</t>
         </is>
       </c>
-      <c r="C2" s="24" t="n">
+      <c r="C2" s="22" t="n">
         <v>546827551</v>
       </c>
       <c r="D2" s="20" t="n">
@@ -2657,11 +2728,13 @@
       <c r="E2" s="20" t="n">
         <v>44037</v>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="5" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="n"/>
@@ -2669,7 +2742,9 @@
       <c r="C3" s="1" t="n"/>
       <c r="D3" s="20" t="n"/>
       <c r="E3" s="20" t="n"/>
-      <c r="F3" s="5" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="n"/>
@@ -2677,7 +2752,9 @@
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="20" t="n"/>
       <c r="E4" s="20" t="n"/>
-      <c r="F4" s="5" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n"/>
@@ -2685,7 +2762,9 @@
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="20" t="n"/>
       <c r="E5" s="20" t="n"/>
-      <c r="F5" s="5" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n"/>
@@ -2693,7 +2772,9 @@
       <c r="C6" s="1" t="n"/>
       <c r="D6" s="20" t="n"/>
       <c r="E6" s="20" t="n"/>
-      <c r="F6" s="5" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n"/>
@@ -2701,7 +2782,9 @@
       <c r="C7" s="1" t="n"/>
       <c r="D7" s="20" t="n"/>
       <c r="E7" s="20" t="n"/>
-      <c r="F7" s="5" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n"/>
@@ -2709,7 +2792,9 @@
       <c r="C8" s="1" t="n"/>
       <c r="D8" s="20" t="n"/>
       <c r="E8" s="20" t="n"/>
-      <c r="F8" s="5" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
@@ -2717,7 +2802,9 @@
       <c r="C9" s="1" t="n"/>
       <c r="D9" s="20" t="n"/>
       <c r="E9" s="20" t="n"/>
-      <c r="F9" s="5" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="5" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="n"/>
@@ -2725,7 +2812,9 @@
       <c r="C10" s="1" t="n"/>
       <c r="D10" s="20" t="n"/>
       <c r="E10" s="20" t="n"/>
-      <c r="F10" s="5" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="5" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n"/>
@@ -2733,7 +2822,9 @@
       <c r="C11" s="1" t="n"/>
       <c r="D11" s="20" t="n"/>
       <c r="E11" s="20" t="n"/>
-      <c r="F11" s="5" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="5" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n"/>
@@ -2741,7 +2832,9 @@
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="20" t="n"/>
       <c r="E12" s="20" t="n"/>
-      <c r="F12" s="5" t="n"/>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n"/>
@@ -2749,7 +2842,9 @@
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="20" t="n"/>
       <c r="E13" s="20" t="n"/>
-      <c r="F13" s="5" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="5" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="n"/>
@@ -2757,7 +2852,9 @@
       <c r="C14" s="1" t="n"/>
       <c r="D14" s="20" t="n"/>
       <c r="E14" s="20" t="n"/>
-      <c r="F14" s="5" t="n"/>
+      <c r="F14" s="1" t="n"/>
+      <c r="G14" s="1" t="n"/>
+      <c r="H14" s="5" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n"/>
@@ -2765,7 +2862,9 @@
       <c r="C15" s="1" t="n"/>
       <c r="D15" s="20" t="n"/>
       <c r="E15" s="20" t="n"/>
-      <c r="F15" s="5" t="n"/>
+      <c r="F15" s="1" t="n"/>
+      <c r="G15" s="1" t="n"/>
+      <c r="H15" s="5" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n"/>
@@ -2773,7 +2872,9 @@
       <c r="C16" s="1" t="n"/>
       <c r="D16" s="20" t="n"/>
       <c r="E16" s="20" t="n"/>
-      <c r="F16" s="5" t="n"/>
+      <c r="F16" s="1" t="n"/>
+      <c r="G16" s="1" t="n"/>
+      <c r="H16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n"/>
@@ -2781,7 +2882,9 @@
       <c r="C17" s="1" t="n"/>
       <c r="D17" s="20" t="n"/>
       <c r="E17" s="20" t="n"/>
-      <c r="F17" s="5" t="n"/>
+      <c r="F17" s="1" t="n"/>
+      <c r="G17" s="1" t="n"/>
+      <c r="H17" s="5" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="n"/>
@@ -2789,7 +2892,9 @@
       <c r="C18" s="1" t="n"/>
       <c r="D18" s="20" t="n"/>
       <c r="E18" s="20" t="n"/>
-      <c r="F18" s="5" t="n"/>
+      <c r="F18" s="1" t="n"/>
+      <c r="G18" s="1" t="n"/>
+      <c r="H18" s="5" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n"/>
@@ -2797,7 +2902,9 @@
       <c r="C19" s="1" t="n"/>
       <c r="D19" s="20" t="n"/>
       <c r="E19" s="20" t="n"/>
-      <c r="F19" s="5" t="n"/>
+      <c r="F19" s="1" t="n"/>
+      <c r="G19" s="1" t="n"/>
+      <c r="H19" s="5" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="n"/>
@@ -2805,7 +2912,9 @@
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="20" t="n"/>
       <c r="E20" s="20" t="n"/>
-      <c r="F20" s="5" t="n"/>
+      <c r="F20" s="1" t="n"/>
+      <c r="G20" s="1" t="n"/>
+      <c r="H20" s="5" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n"/>
@@ -2813,7 +2922,9 @@
       <c r="C21" s="1" t="n"/>
       <c r="D21" s="20" t="n"/>
       <c r="E21" s="20" t="n"/>
-      <c r="F21" s="5" t="n"/>
+      <c r="F21" s="1" t="n"/>
+      <c r="G21" s="1" t="n"/>
+      <c r="H21" s="5" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="n"/>
@@ -2821,7 +2932,9 @@
       <c r="C22" s="1" t="n"/>
       <c r="D22" s="20" t="n"/>
       <c r="E22" s="20" t="n"/>
-      <c r="F22" s="5" t="n"/>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" s="1" t="n"/>
+      <c r="H22" s="5" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n"/>
@@ -2829,7 +2942,9 @@
       <c r="C23" s="1" t="n"/>
       <c r="D23" s="20" t="n"/>
       <c r="E23" s="20" t="n"/>
-      <c r="F23" s="5" t="n"/>
+      <c r="F23" s="1" t="n"/>
+      <c r="G23" s="1" t="n"/>
+      <c r="H23" s="5" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="n"/>
@@ -2837,7 +2952,9 @@
       <c r="C24" s="1" t="n"/>
       <c r="D24" s="20" t="n"/>
       <c r="E24" s="20" t="n"/>
-      <c r="F24" s="5" t="n"/>
+      <c r="F24" s="1" t="n"/>
+      <c r="G24" s="1" t="n"/>
+      <c r="H24" s="5" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n"/>
@@ -2845,7 +2962,9 @@
       <c r="C25" s="1" t="n"/>
       <c r="D25" s="20" t="n"/>
       <c r="E25" s="20" t="n"/>
-      <c r="F25" s="5" t="n"/>
+      <c r="F25" s="1" t="n"/>
+      <c r="G25" s="1" t="n"/>
+      <c r="H25" s="5" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n"/>
@@ -2853,7 +2972,9 @@
       <c r="C26" s="1" t="n"/>
       <c r="D26" s="20" t="n"/>
       <c r="E26" s="20" t="n"/>
-      <c r="F26" s="5" t="n"/>
+      <c r="F26" s="1" t="n"/>
+      <c r="G26" s="1" t="n"/>
+      <c r="H26" s="5" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="27" thickBot="1">
       <c r="A27" s="6" t="n"/>
@@ -2861,7 +2982,9 @@
       <c r="C27" s="7" t="n"/>
       <c r="D27" s="21" t="n"/>
       <c r="E27" s="21" t="n"/>
-      <c r="F27" s="8" t="n"/>
+      <c r="F27" s="7" t="n"/>
+      <c r="G27" s="7" t="n"/>
+      <c r="H27" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2875,60 +2998,73 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="9.85546875"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="9.42578125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="10.5703125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10.28515625"/>
     <col bestFit="1" customWidth="1" max="3" min="3" width="10"/>
-    <col bestFit="1" customWidth="1" max="5" min="4" width="17.28515625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="10.85546875"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="10"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="15"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="13.5703125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="20.5703125"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row customHeight="1" ht="15.75" r="1">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>Firstname</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>Lastname</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>Birth date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Test date</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>Patient Status</t>
         </is>
       </c>
+      <c r="G1" s="12" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="H1" s="19" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Mike</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>lasto</t>
         </is>
@@ -2936,97 +3072,349 @@
       <c r="C2" s="22" t="n">
         <v>546827551</v>
       </c>
-      <c r="D2" s="23" t="n">
+      <c r="D2" s="20" t="n">
         <v>35028</v>
       </c>
-      <c r="E2" s="23" t="n">
+      <c r="E2" s="20" t="n">
         <v>44037</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="5" t="n"/>
     </row>
     <row r="3">
-      <c r="D3" s="23" t="n"/>
-      <c r="E3" s="23" t="n"/>
+      <c r="A3" s="4" t="n"/>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="20" t="n"/>
+      <c r="E3" s="20" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="4">
-      <c r="D4" s="23" t="n"/>
-      <c r="E4" s="23" t="n"/>
+      <c r="A4" s="4" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="20" t="n"/>
+      <c r="E4" s="20" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="5" t="n"/>
     </row>
     <row r="5">
-      <c r="D5" s="23" t="n"/>
-      <c r="E5" s="23" t="n"/>
+      <c r="A5" s="4" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="20" t="n"/>
+      <c r="E5" s="20" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="5" t="n"/>
     </row>
     <row r="6">
-      <c r="D6" s="23" t="n"/>
-      <c r="E6" s="23" t="n"/>
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="20" t="n"/>
+      <c r="E6" s="20" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="5" t="n"/>
     </row>
     <row r="7">
-      <c r="D7" s="23" t="n"/>
-      <c r="E7" s="23" t="n"/>
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="20" t="n"/>
+      <c r="E7" s="20" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="D8" s="23" t="n"/>
-      <c r="E8" s="23" t="n"/>
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="20" t="n"/>
+      <c r="E8" s="20" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="D9" s="23" t="n"/>
-      <c r="E9" s="23" t="n"/>
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="20" t="n"/>
+      <c r="E9" s="20" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="5" t="n"/>
     </row>
     <row r="10">
-      <c r="D10" s="23" t="n"/>
-      <c r="E10" s="23" t="n"/>
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="20" t="n"/>
+      <c r="E10" s="20" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="5" t="n"/>
     </row>
     <row r="11">
-      <c r="D11" s="23" t="n"/>
-      <c r="E11" s="23" t="n"/>
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="20" t="n"/>
+      <c r="E11" s="20" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="5" t="n"/>
     </row>
     <row r="12">
-      <c r="D12" s="23" t="n"/>
-      <c r="E12" s="23" t="n"/>
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="20" t="n"/>
+      <c r="E12" s="20" t="n"/>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" s="1" t="n"/>
+      <c r="H12" s="5" t="n"/>
     </row>
     <row r="13">
-      <c r="D13" s="23" t="n"/>
-      <c r="E13" s="23" t="n"/>
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="20" t="n"/>
+      <c r="E13" s="20" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" s="1" t="n"/>
+      <c r="H13" s="5" t="n"/>
     </row>
     <row r="14">
-      <c r="D14" s="23" t="n"/>
-      <c r="E14" s="23" t="n"/>
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="20" t="n"/>
+      <c r="E14" s="20" t="n"/>
+      <c r="F14" s="1" t="n"/>
+      <c r="G14" s="1" t="n"/>
+      <c r="H14" s="5" t="n"/>
     </row>
     <row r="15">
-      <c r="D15" s="23" t="n"/>
-      <c r="E15" s="23" t="n"/>
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
+      <c r="D15" s="20" t="n"/>
+      <c r="E15" s="20" t="n"/>
+      <c r="F15" s="1" t="n"/>
+      <c r="G15" s="1" t="n"/>
+      <c r="H15" s="5" t="n"/>
     </row>
     <row r="16">
-      <c r="D16" s="23" t="n"/>
-      <c r="E16" s="23" t="n"/>
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="20" t="n"/>
+      <c r="E16" s="20" t="n"/>
+      <c r="F16" s="1" t="n"/>
+      <c r="G16" s="1" t="n"/>
+      <c r="H16" s="5" t="n"/>
     </row>
     <row r="17">
-      <c r="D17" s="23" t="n"/>
-      <c r="E17" s="23" t="n"/>
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="20" t="n"/>
+      <c r="E17" s="20" t="n"/>
+      <c r="F17" s="1" t="n"/>
+      <c r="G17" s="1" t="n"/>
+      <c r="H17" s="5" t="n"/>
     </row>
     <row r="18">
-      <c r="D18" s="23" t="n"/>
-      <c r="E18" s="23" t="n"/>
+      <c r="A18" s="4" t="n"/>
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="n"/>
+      <c r="D18" s="20" t="n"/>
+      <c r="E18" s="20" t="n"/>
+      <c r="F18" s="1" t="n"/>
+      <c r="G18" s="1" t="n"/>
+      <c r="H18" s="5" t="n"/>
     </row>
     <row r="19">
-      <c r="D19" s="23" t="n"/>
-      <c r="E19" s="23" t="n"/>
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="1" t="n"/>
+      <c r="C19" s="1" t="n"/>
+      <c r="D19" s="20" t="n"/>
+      <c r="E19" s="20" t="n"/>
+      <c r="F19" s="1" t="n"/>
+      <c r="G19" s="1" t="n"/>
+      <c r="H19" s="5" t="n"/>
     </row>
     <row r="20">
-      <c r="D20" s="23" t="n"/>
-      <c r="E20" s="23" t="n"/>
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="20" t="n"/>
+      <c r="E20" s="20" t="n"/>
+      <c r="F20" s="1" t="n"/>
+      <c r="G20" s="1" t="n"/>
+      <c r="H20" s="5" t="n"/>
     </row>
     <row r="21">
-      <c r="D21" s="23" t="n"/>
-      <c r="E21" s="23" t="n"/>
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="20" t="n"/>
+      <c r="E21" s="20" t="n"/>
+      <c r="F21" s="1" t="n"/>
+      <c r="G21" s="1" t="n"/>
+      <c r="H21" s="5" t="n"/>
     </row>
     <row r="22">
-      <c r="D22" s="23" t="n"/>
-      <c r="E22" s="23" t="n"/>
+      <c r="A22" s="4" t="n"/>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="20" t="n"/>
+      <c r="E22" s="20" t="n"/>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" s="1" t="n"/>
+      <c r="H22" s="5" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="n"/>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
+      <c r="F23" s="1" t="n"/>
+      <c r="G23" s="1" t="n"/>
+      <c r="H23" s="5" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="n"/>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
+      <c r="F24" s="1" t="n"/>
+      <c r="G24" s="1" t="n"/>
+      <c r="H24" s="5" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="n"/>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="1" t="n"/>
+      <c r="D25" s="1" t="n"/>
+      <c r="E25" s="1" t="n"/>
+      <c r="F25" s="1" t="n"/>
+      <c r="G25" s="1" t="n"/>
+      <c r="H25" s="5" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="n"/>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
+      <c r="D26" s="1" t="n"/>
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
+      <c r="G26" s="1" t="n"/>
+      <c r="H26" s="5" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="n"/>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="n"/>
+      <c r="D27" s="1" t="n"/>
+      <c r="E27" s="1" t="n"/>
+      <c r="F27" s="1" t="n"/>
+      <c r="G27" s="1" t="n"/>
+      <c r="H27" s="5" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="n"/>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="1" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
+      <c r="F28" s="1" t="n"/>
+      <c r="G28" s="1" t="n"/>
+      <c r="H28" s="5" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
+      <c r="E29" s="1" t="n"/>
+      <c r="F29" s="1" t="n"/>
+      <c r="G29" s="1" t="n"/>
+      <c r="H29" s="5" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="n"/>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
+      <c r="G30" s="1" t="n"/>
+      <c r="H30" s="5" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="1" t="n"/>
+      <c r="C31" s="1" t="n"/>
+      <c r="D31" s="1" t="n"/>
+      <c r="E31" s="1" t="n"/>
+      <c r="F31" s="1" t="n"/>
+      <c r="G31" s="1" t="n"/>
+      <c r="H31" s="5" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="1" t="n"/>
+      <c r="C32" s="1" t="n"/>
+      <c r="D32" s="1" t="n"/>
+      <c r="E32" s="1" t="n"/>
+      <c r="F32" s="1" t="n"/>
+      <c r="G32" s="1" t="n"/>
+      <c r="H32" s="5" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="n"/>
+      <c r="B33" s="1" t="n"/>
+      <c r="C33" s="1" t="n"/>
+      <c r="D33" s="1" t="n"/>
+      <c r="E33" s="1" t="n"/>
+      <c r="F33" s="1" t="n"/>
+      <c r="G33" s="1" t="n"/>
+      <c r="H33" s="5" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="n"/>
+      <c r="B34" s="1" t="n"/>
+      <c r="C34" s="1" t="n"/>
+      <c r="D34" s="1" t="n"/>
+      <c r="E34" s="1" t="n"/>
+      <c r="F34" s="1" t="n"/>
+      <c r="G34" s="1" t="n"/>
+      <c r="H34" s="5" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="35" thickBot="1">
+      <c r="A35" s="6" t="n"/>
+      <c r="B35" s="7" t="n"/>
+      <c r="C35" s="7" t="n"/>
+      <c r="D35" s="7" t="n"/>
+      <c r="E35" s="7" t="n"/>
+      <c r="F35" s="7" t="n"/>
+      <c r="G35" s="7" t="n"/>
+      <c r="H35" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -3040,13 +3428,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="3" min="3" width="17.42578125"/>
+    <col customWidth="1" max="4" min="4" width="19.42578125"/>
+    <col customWidth="1" max="5" min="5" width="18.140625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="12.140625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" width="18.5703125"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -3079,157 +3475,56 @@
           <t>Patient Status</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Quarantined</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Where quarantined</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>Johnny</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tghg</t>
-        </is>
-      </c>
-      <c r="C2" s="22" t="n">
-        <v>458725418</v>
-      </c>
-      <c r="D2" s="27" t="n">
-        <v>35055</v>
-      </c>
-      <c r="E2" s="27" t="n">
-        <v>44057</v>
+          <t>Bravo</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>544327551</v>
+      </c>
+      <c r="D2" s="26" t="n">
+        <v>36020</v>
+      </c>
+      <c r="E2" s="26" t="n">
+        <v>44037</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Active</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Leonardo Hotel</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="C3" s="22" t="n"/>
-      <c r="D3" s="27" t="n"/>
-      <c r="E3" s="27" t="n"/>
-    </row>
-    <row r="4">
-      <c r="C4" s="22" t="n"/>
-      <c r="D4" s="27" t="n"/>
-      <c r="E4" s="27" t="n"/>
-    </row>
-    <row r="5">
-      <c r="C5" s="22" t="n"/>
-      <c r="D5" s="27" t="n"/>
-      <c r="E5" s="27" t="n"/>
-    </row>
-    <row r="6">
-      <c r="C6" s="22" t="n"/>
-      <c r="D6" s="27" t="n"/>
-      <c r="E6" s="27" t="n"/>
-    </row>
-    <row r="7">
-      <c r="C7" s="22" t="n"/>
-      <c r="D7" s="27" t="n"/>
-      <c r="E7" s="27" t="n"/>
-    </row>
-    <row r="8">
-      <c r="C8" s="22" t="n"/>
-      <c r="D8" s="27" t="n"/>
-      <c r="E8" s="27" t="n"/>
-    </row>
-    <row r="9">
-      <c r="C9" s="22" t="n"/>
-      <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="n"/>
-    </row>
-    <row r="10">
-      <c r="C10" s="22" t="n"/>
-      <c r="D10" s="27" t="n"/>
-      <c r="E10" s="27" t="n"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="22" t="n"/>
-      <c r="D11" s="27" t="n"/>
-      <c r="E11" s="27" t="n"/>
-    </row>
-    <row r="12">
-      <c r="C12" s="22" t="n"/>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
-    </row>
-    <row r="13">
-      <c r="C13" s="22" t="n"/>
-      <c r="D13" s="27" t="n"/>
-      <c r="E13" s="27" t="n"/>
-    </row>
-    <row r="14">
-      <c r="C14" s="22" t="n"/>
-      <c r="D14" s="27" t="n"/>
-      <c r="E14" s="27" t="n"/>
-    </row>
-    <row r="15">
-      <c r="C15" s="22" t="n"/>
-      <c r="D15" s="27" t="n"/>
-      <c r="E15" s="27" t="n"/>
-    </row>
-    <row r="16">
-      <c r="C16" s="22" t="n"/>
-      <c r="D16" s="27" t="n"/>
-      <c r="E16" s="27" t="n"/>
-    </row>
-    <row r="17">
-      <c r="C17" s="22" t="n"/>
-      <c r="D17" s="27" t="n"/>
-      <c r="E17" s="27" t="n"/>
-    </row>
-    <row r="18">
-      <c r="C18" s="22" t="n"/>
-      <c r="D18" s="27" t="n"/>
-      <c r="E18" s="27" t="n"/>
-    </row>
-    <row r="19">
-      <c r="C19" s="22" t="n"/>
-      <c r="D19" s="27" t="n"/>
-      <c r="E19" s="27" t="n"/>
-    </row>
-    <row r="20">
-      <c r="C20" s="22" t="n"/>
-      <c r="D20" s="27" t="n"/>
-      <c r="E20" s="27" t="n"/>
-    </row>
-    <row r="21">
-      <c r="C21" s="22" t="n"/>
-      <c r="D21" s="27" t="n"/>
-      <c r="E21" s="27" t="n"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="22" t="n"/>
-      <c r="D22" s="27" t="n"/>
-      <c r="E22" s="27" t="n"/>
-    </row>
-    <row r="23">
-      <c r="C23" s="22" t="n"/>
-      <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
-    </row>
-    <row r="24">
-      <c r="C24" s="22" t="n"/>
-      <c r="D24" s="27" t="n"/>
-      <c r="E24" s="27" t="n"/>
-    </row>
-    <row r="25">
-      <c r="C25" s="22" t="n"/>
-      <c r="D25" s="27" t="n"/>
-      <c r="E25" s="27" t="n"/>
-    </row>
-    <row r="26">
-      <c r="C26" s="22" t="n"/>
-      <c r="D26" s="27" t="n"/>
-      <c r="E26" s="27" t="n"/>
-    </row>
-    <row r="27">
-      <c r="C27" s="22" t="n"/>
-      <c r="D27" s="27" t="n"/>
-      <c r="E27" s="27" t="n"/>
+      <c r="D3" s="26" t="n"/>
+      <c r="E3" s="26" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Created AddPatientToDBTkinter.py Same as AddPatientToDB.py but in Tkinter (a lot easier now)
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -17,14 +17,13 @@
     <sheet name="Tel Aviv-Yafo" sheetId="3" r:id="rId3"/>
     <sheet name="Ashdod" sheetId="4" r:id="rId4"/>
     <sheet name="Lod" sheetId="5" r:id="rId5"/>
-    <sheet name="Tamar" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
   <si>
     <t>City</t>
   </si>
@@ -333,10 +332,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -563,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -612,8 +610,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,7 +893,7 @@
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2354,7 +2350,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H27"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3424,7 +3420,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3496,194 +3492,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="26">
-        <v>544327551</v>
-      </c>
-      <c r="D2" s="27">
-        <v>36020</v>
-      </c>
-      <c r="E2" s="27">
-        <v>44037</v>
-      </c>
-      <c r="F2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-    </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-    </row>
-    <row r="18" spans="3:5">
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-    </row>
-    <row r="19" spans="3:5">
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-    </row>
-    <row r="20" spans="3:5">
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-    </row>
-    <row r="21" spans="3:5">
-      <c r="C21" s="26"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-    </row>
-    <row r="22" spans="3:5">
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-    </row>
-    <row r="23" spans="3:5">
-      <c r="C23" s="26"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-    </row>
-    <row r="24" spans="3:5">
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-    </row>
-    <row r="25" spans="3:5">
-      <c r="C25" s="26"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="3:5">
-      <c r="C26" s="26"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-    </row>
-    <row r="27" spans="3:5">
-      <c r="C27" s="26"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added main page for now all the other windows turn on too
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sman9\Desktop\Git Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -331,7 +331,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
@@ -892,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3419,7 +3419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added in ReportsTkinter.py "find by id" and "find by name" by name doesn't work for now
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sman9\Desktop\Git Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
   <si>
     <t>City</t>
   </si>
@@ -326,12 +326,18 @@
   </si>
   <si>
     <t>Leonardo Hotel</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Hotel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
@@ -2349,8 +2355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2416,8 +2422,12 @@
       <c r="F2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="5"/>
+      <c r="G2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
@@ -2438,8 +2448,12 @@
       <c r="F3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="4"/>
@@ -3419,8 +3433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>